<commit_message>
add new speedup figure and final report
</commit_message>
<xml_diff>
--- a/project5/Workbook1.xlsx
+++ b/project5/Workbook1.xlsx
@@ -478,11 +478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="249626176"/>
-        <c:axId val="332793040"/>
+        <c:axId val="-474644592"/>
+        <c:axId val="-474640560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="249626176"/>
+        <c:axId val="-474644592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +606,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332793040"/>
+        <c:crossAx val="-474640560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,7 +614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332793040"/>
+        <c:axId val="-474640560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +730,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249626176"/>
+        <c:crossAx val="-474644592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1178,11 +1178,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="332818176"/>
-        <c:axId val="332821936"/>
+        <c:axId val="-474604672"/>
+        <c:axId val="-474600912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332818176"/>
+        <c:axId val="-474604672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1306,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332821936"/>
+        <c:crossAx val="-474600912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1314,7 +1314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332821936"/>
+        <c:axId val="-474600912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1429,7 +1429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332818176"/>
+        <c:crossAx val="-474604672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2086,11 +2086,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="332867168"/>
-        <c:axId val="332870928"/>
+        <c:axId val="-474555344"/>
+        <c:axId val="-474551584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332867168"/>
+        <c:axId val="-474555344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2213,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332870928"/>
+        <c:crossAx val="-474551584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2221,7 +2221,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332870928"/>
+        <c:axId val="-474551584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,7 +2337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332867168"/>
+        <c:crossAx val="-474555344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2994,11 +2994,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="288538928"/>
-        <c:axId val="288542336"/>
+        <c:axId val="-513264432"/>
+        <c:axId val="-513261360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288538928"/>
+        <c:axId val="-513264432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3122,7 +3122,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288542336"/>
+        <c:crossAx val="-513261360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3130,7 +3130,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288542336"/>
+        <c:axId val="-513261360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3246,7 +3246,727 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288538928"/>
+        <c:crossAx val="-513264432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Speedup</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>SIMD</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>over</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>Non-SIMD</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1 Thread</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16M</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32M</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48M</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.805146742404682</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.952594586511141</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.420642893018584</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.911832839140104</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.06815180065158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.809888357256778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2 Threads</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16M</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32M</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48M</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.956476250261561</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.912</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.133713521090863</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.393922234805587</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.938818202659331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.402801292904417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>4 Threads</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16M</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32M</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48M</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.487422680412371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.136790739900136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.874394456989558</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.502618986032075</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.593226017453455</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.498765588402862</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.940207453181159</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-383902800"/>
+        <c:axId val="-383886496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-383902800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Data</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t>Set</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t>Size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t>(NUMS)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-383886496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-383886496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-383902800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3487,6 +4207,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4997,6 +5757,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5504,15 +6767,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>295910</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>115570</xdr:rowOff>
+      <xdr:colOff>319429</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>186126</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>353060</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>147320</xdr:rowOff>
+      <xdr:colOff>376579</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>14049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5533,16 +6796,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>792480</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>142240</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>72186</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>41580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>173990</xdr:rowOff>
+      <xdr:colOff>136109</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>73330</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5622,6 +6885,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>397933</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>474133</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>16932</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5893,10 +7186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="R11" zoomScale="167" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6083,6 +7376,93 @@
         <v>2499.5100000000002</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" ref="B9:H9" si="0">B5/B2</f>
+        <v>3.8051467424046823</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>3.9525945865111409</v>
+      </c>
+      <c r="D9">
+        <v>3.89</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3.4206428930185839</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.9118328391401036</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3.0681518006515804</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>2.8098883572567783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f t="shared" ref="B10:H10" si="1">B6/B3</f>
+        <v>2.9564762502615607</v>
+      </c>
+      <c r="C10">
+        <v>3.9119999999999999</v>
+      </c>
+      <c r="D10">
+        <v>3.9</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>3.1337135210908627</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3.3939222348055869</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>2.9388182026593306</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3.4028012929044174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f>B7/B4</f>
+        <v>1.4874226804123711</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:H11" si="2">C7/C4</f>
+        <v>3.1367907399001358</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>2.8743944569895583</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>2.5026189860320747</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>2.5932260174534552</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>3.4987655884028617</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>3.9402074531811593</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
final version of project 5
</commit_message>
<xml_diff>
--- a/project5/Workbook1.xlsx
+++ b/project5/Workbook1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -47,12 +47,6 @@
     <t>10K</t>
   </si>
   <si>
-    <t>16M</t>
-  </si>
-  <si>
-    <t>48M</t>
-  </si>
-  <si>
     <t>1(NON-VEC)</t>
   </si>
   <si>
@@ -61,15 +55,37 @@
   <si>
     <t>4(NON-VEC)</t>
   </si>
+  <si>
+    <t>128M</t>
+  </si>
+  <si>
+    <t>256M</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,13 +108,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -240,16 +264,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -261,25 +285,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>116.19</c:v>
+                  <c:v>121.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>133.74</c:v>
+                  <c:v>132.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140.51</c:v>
+                  <c:v>140.21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>159.28</c:v>
+                  <c:v>209.74</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>215.84</c:v>
+                  <c:v>235.56</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>227.14</c:v>
+                  <c:v>284.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>250.8</c:v>
+                  <c:v>356.49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -331,16 +355,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -352,25 +376,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>191.16</c:v>
+                  <c:v>188.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>252.93</c:v>
+                  <c:v>222.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>269.82</c:v>
+                  <c:v>267.58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>313.88</c:v>
+                  <c:v>318.49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>317.88</c:v>
+                  <c:v>372.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>348.96</c:v>
+                  <c:v>378.24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>324.85</c:v>
+                  <c:v>542.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,16 +446,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -443,25 +467,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>169.75</c:v>
+                  <c:v>239.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>440.6</c:v>
+                  <c:v>268.72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>518.13</c:v>
+                  <c:v>440.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>618.5599999999999</c:v>
+                  <c:v>624.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>626.8099999999999</c:v>
+                  <c:v>683.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>631.88</c:v>
+                  <c:v>772.39</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>634.36</c:v>
+                  <c:v>927.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,11 +502,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-474644592"/>
-        <c:axId val="-474640560"/>
+        <c:axId val="122825168"/>
+        <c:axId val="122828784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-474644592"/>
+        <c:axId val="122825168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-474640560"/>
+        <c:crossAx val="122828784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,7 +638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-474640560"/>
+        <c:axId val="122828784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-474644592"/>
+        <c:crossAx val="122825168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -940,16 +964,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -964,22 +988,22 @@
                   <c:v>442.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>528.62</c:v>
+                  <c:v>516.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>596.49</c:v>
+                  <c:v>594.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>544.84</c:v>
+                  <c:v>695.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>628.49</c:v>
+                  <c:v>710.46</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>696.9</c:v>
+                  <c:v>865.17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>704.72</c:v>
+                  <c:v>1062.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1031,16 +1055,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1052,25 +1076,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>565.16</c:v>
+                  <c:v>457.23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1023.75</c:v>
+                  <c:v>937.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1181.69</c:v>
+                  <c:v>1148.89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>983.61</c:v>
+                  <c:v>1159.87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1078.86</c:v>
+                  <c:v>1160.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1025.53</c:v>
+                  <c:v>1105.07</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1105.4</c:v>
+                  <c:v>1275.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1122,16 +1146,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1143,25 +1167,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>252.49</c:v>
+                  <c:v>236.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1382.07</c:v>
+                  <c:v>1023.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1489.31</c:v>
+                  <c:v>1784.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1548.02</c:v>
+                  <c:v>2236.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1625.46</c:v>
+                  <c:v>2409.53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2210.8</c:v>
+                  <c:v>2577.42</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2499.51</c:v>
+                  <c:v>2855.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1178,11 +1202,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-474604672"/>
-        <c:axId val="-474600912"/>
+        <c:axId val="122858864"/>
+        <c:axId val="122862624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-474604672"/>
+        <c:axId val="122858864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-474600912"/>
+        <c:crossAx val="122862624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1314,7 +1338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-474600912"/>
+        <c:axId val="122862624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1429,7 +1453,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-474604672"/>
+        <c:crossAx val="122858864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1649,13 +1673,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>116.19</c:v>
+                  <c:v>121.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>191.16</c:v>
+                  <c:v>188.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>169.75</c:v>
+                  <c:v>239.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,13 +1741,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>133.74</c:v>
+                  <c:v>132.65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>252.93</c:v>
+                  <c:v>222.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>440.6</c:v>
+                  <c:v>268.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1785,13 +1809,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>140.51</c:v>
+                  <c:v>140.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>269.82</c:v>
+                  <c:v>267.58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>518.13</c:v>
+                  <c:v>440.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1802,7 +1826,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>16M</c:v>
+            <c:v>32M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1853,13 +1877,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>159.28</c:v>
+                  <c:v>209.74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>313.88</c:v>
+                  <c:v>318.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>618.5599999999999</c:v>
+                  <c:v>624.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1870,7 +1894,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>32M</c:v>
+            <c:v>64M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1921,13 +1945,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>215.84</c:v>
+                  <c:v>235.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>317.88</c:v>
+                  <c:v>372.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>626.8099999999999</c:v>
+                  <c:v>683.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1938,7 +1962,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>48M</c:v>
+            <c:v>128M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1989,13 +2013,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>227.14</c:v>
+                  <c:v>284.76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>348.96</c:v>
+                  <c:v>378.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>631.88</c:v>
+                  <c:v>772.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2006,7 +2030,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>64M</c:v>
+            <c:v>256M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2063,13 +2087,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>250.8</c:v>
+                  <c:v>356.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>324.85</c:v>
+                  <c:v>542.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>634.36</c:v>
+                  <c:v>927.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2086,11 +2110,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-474555344"/>
-        <c:axId val="-474551584"/>
+        <c:axId val="122913312"/>
+        <c:axId val="120985136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-474555344"/>
+        <c:axId val="122913312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2237,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-474551584"/>
+        <c:crossAx val="120985136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2221,7 +2245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-474551584"/>
+        <c:axId val="120985136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,7 +2361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-474555344"/>
+        <c:crossAx val="122913312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2560,10 +2584,10 @@
                   <c:v>442.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>565.16</c:v>
+                  <c:v>457.23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>252.49</c:v>
+                  <c:v>236.68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2625,13 +2649,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>528.62</c:v>
+                  <c:v>516.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1023.75</c:v>
+                  <c:v>937.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1382.07</c:v>
+                  <c:v>1023.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2693,13 +2717,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>596.49</c:v>
+                  <c:v>594.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1181.69</c:v>
+                  <c:v>1148.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1489.31</c:v>
+                  <c:v>1784.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,7 +2734,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>16M</c:v>
+            <c:v>32M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2761,13 +2785,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>544.84</c:v>
+                  <c:v>695.24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>983.61</c:v>
+                  <c:v>1159.87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1548.02</c:v>
+                  <c:v>2236.66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2778,7 +2802,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>32M</c:v>
+            <c:v>64M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2829,13 +2853,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>628.49</c:v>
+                  <c:v>710.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1078.86</c:v>
+                  <c:v>1160.03</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1625.46</c:v>
+                  <c:v>2409.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2846,7 +2870,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>48M</c:v>
+            <c:v>128M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2897,13 +2921,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>696.9</c:v>
+                  <c:v>865.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1025.53</c:v>
+                  <c:v>1105.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2210.8</c:v>
+                  <c:v>2577.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2914,7 +2938,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>64M</c:v>
+            <c:v>256M</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2971,13 +2995,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>704.72</c:v>
+                  <c:v>1062.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1105.4</c:v>
+                  <c:v>1275.17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2499.51</c:v>
+                  <c:v>2855.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2994,11 +3018,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-513264432"/>
-        <c:axId val="-513261360"/>
+        <c:axId val="121062944"/>
+        <c:axId val="121066288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-513264432"/>
+        <c:axId val="121062944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3122,7 +3146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-513261360"/>
+        <c:crossAx val="121066288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3130,7 +3154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-513261360"/>
+        <c:axId val="121066288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3246,7 +3270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-513264432"/>
+        <c:crossAx val="121062944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3485,16 +3509,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3506,25 +3530,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.805146742404682</c:v>
+                  <c:v>3.637051661730832</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.952594586511141</c:v>
+                  <c:v>3.89280060309084</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.420642893018584</c:v>
+                  <c:v>3.314770668446648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.911832839140104</c:v>
+                  <c:v>3.016046867040245</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.06815180065158</c:v>
+                  <c:v>3.038242730720607</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.809888357256778</c:v>
+                  <c:v>2.980476310695952</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3576,16 +3600,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3597,7 +3621,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.956476250261561</c:v>
+                  <c:v>2.431169245493699</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.912</c:v>
@@ -3606,16 +3630,16 @@
                   <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.133713521090863</c:v>
+                  <c:v>3.641778391786241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.393922234805587</c:v>
+                  <c:v>3.118276390419612</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.938818202659331</c:v>
+                  <c:v>2.921610617597293</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.402801292904417</c:v>
+                  <c:v>2.350067267466505</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3667,16 +3691,16 @@
                   <c:v>100K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16M</c:v>
+                  <c:v>32M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32M</c:v>
+                  <c:v>64M</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48M</c:v>
+                  <c:v>128M</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64M</c:v>
+                  <c:v>256M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3688,25 +3712,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.487422680412371</c:v>
+                  <c:v>0.990251453914062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.136790739900136</c:v>
+                  <c:v>3.809020541827924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.874394456989558</c:v>
+                  <c:v>4.052551495469307</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.502618986032075</c:v>
+                  <c:v>3.584276144995352</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.593226017453455</c:v>
+                  <c:v>3.523631949928344</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.498765588402862</c:v>
+                  <c:v>3.336941182563213</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.940207453181159</c:v>
+                  <c:v>3.079577685032407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3723,11 +3747,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-383902800"/>
-        <c:axId val="-383886496"/>
+        <c:axId val="122924912"/>
+        <c:axId val="122928672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-383902800"/>
+        <c:axId val="122924912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3851,7 +3875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-383886496"/>
+        <c:crossAx val="122928672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3859,7 +3883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-383886496"/>
+        <c:axId val="122928672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3966,7 +3990,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-383902800"/>
+        <c:crossAx val="122924912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7188,8 +7212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R11" zoomScale="167" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7208,94 +7232,94 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>116.19</v>
+        <v>121.56</v>
       </c>
       <c r="C2">
-        <v>133.74</v>
+        <v>132.65</v>
       </c>
       <c r="D2">
-        <v>140.51</v>
+        <v>140.21</v>
       </c>
       <c r="E2">
-        <v>159.28</v>
+        <v>209.74</v>
       </c>
       <c r="F2">
-        <v>215.84</v>
+        <v>235.56</v>
       </c>
       <c r="G2">
-        <v>227.14</v>
+        <v>284.76</v>
       </c>
       <c r="H2">
-        <v>250.8</v>
+        <v>356.49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>191.16</v>
+        <v>188.07</v>
       </c>
       <c r="C3">
-        <v>252.93</v>
+        <v>222.35</v>
       </c>
       <c r="D3">
-        <v>269.82</v>
+        <v>267.58</v>
       </c>
       <c r="E3">
-        <v>313.88</v>
+        <v>318.49</v>
       </c>
       <c r="F3">
-        <v>317.88</v>
+        <v>372.01</v>
       </c>
       <c r="G3">
-        <v>348.96</v>
+        <v>378.24</v>
       </c>
       <c r="H3">
-        <v>324.85000000000002</v>
+        <v>542.61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>169.75</v>
+        <v>239.01</v>
       </c>
       <c r="C4">
-        <v>440.6</v>
+        <v>268.72000000000003</v>
       </c>
       <c r="D4">
-        <v>518.13</v>
+        <v>440.33</v>
       </c>
       <c r="E4">
-        <v>618.55999999999995</v>
+        <v>624.02</v>
       </c>
       <c r="F4">
-        <v>626.80999999999995</v>
+        <v>683.82</v>
       </c>
       <c r="G4">
-        <v>631.88</v>
+        <v>772.39</v>
       </c>
       <c r="H4">
-        <v>634.36</v>
+        <v>927.27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -7306,22 +7330,22 @@
         <v>442.12</v>
       </c>
       <c r="C5">
-        <v>528.62</v>
+        <v>516.38</v>
       </c>
       <c r="D5">
-        <v>596.49</v>
+        <v>594.6</v>
       </c>
       <c r="E5">
-        <v>544.84</v>
+        <v>695.24</v>
       </c>
       <c r="F5">
-        <v>628.49</v>
+        <v>710.46</v>
       </c>
       <c r="G5">
-        <v>696.9</v>
+        <v>865.17</v>
       </c>
       <c r="H5">
-        <v>704.72</v>
+        <v>1062.51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -7329,25 +7353,25 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>565.16</v>
+        <v>457.23</v>
       </c>
       <c r="C6">
-        <v>1023.75</v>
+        <v>937.9</v>
       </c>
       <c r="D6">
-        <v>1181.69</v>
+        <v>1148.8900000000001</v>
       </c>
       <c r="E6">
-        <v>983.61</v>
+        <v>1159.8699999999999</v>
       </c>
       <c r="F6">
-        <v>1078.8599999999999</v>
+        <v>1160.03</v>
       </c>
       <c r="G6">
-        <v>1025.53</v>
+        <v>1105.07</v>
       </c>
       <c r="H6">
-        <v>1105.4000000000001</v>
+        <v>1275.17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -7355,60 +7379,60 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>252.49</v>
+        <v>236.68</v>
       </c>
       <c r="C7">
-        <v>1382.07</v>
+        <v>1023.56</v>
       </c>
       <c r="D7">
-        <v>1489.31</v>
+        <v>1784.46</v>
       </c>
       <c r="E7">
-        <v>1548.02</v>
+        <v>2236.66</v>
       </c>
       <c r="F7">
-        <v>1625.46</v>
+        <v>2409.5300000000002</v>
       </c>
       <c r="G7">
-        <v>2210.8000000000002</v>
+        <v>2577.42</v>
       </c>
       <c r="H7">
-        <v>2499.5100000000002</v>
+        <v>2855.6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9">
-        <f t="shared" ref="B9:H9" si="0">B5/B2</f>
-        <v>3.8051467424046823</v>
+        <f t="shared" ref="B9:G9" si="0">B5/B2</f>
+        <v>3.6370516617308324</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>3.9525945865111409</v>
+        <v>3.8928006030908402</v>
       </c>
       <c r="D9">
         <v>3.89</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>3.4206428930185839</v>
+        <v>3.314770668446648</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>2.9118328391401036</v>
+        <v>3.0160468670402447</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.0681518006515804</v>
+        <v>3.0382427307206066</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>2.8098883572567783</v>
+        <f>H5/H2</f>
+        <v>2.980476310695952</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" ref="B10:H10" si="1">B6/B3</f>
-        <v>2.9564762502615607</v>
+        <v>2.4311692454936993</v>
       </c>
       <c r="C10">
         <v>3.9119999999999999</v>
@@ -7418,49 +7442,49 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>3.1337135210908627</v>
+        <v>3.6417783917862407</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>3.3939222348055869</v>
+        <v>3.1182763904196125</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>2.9388182026593306</v>
+        <v>2.9216106175972927</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>3.4028012929044174</v>
+        <v>2.3500672674665046</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11">
         <f>B7/B4</f>
-        <v>1.4874226804123711</v>
+        <v>0.99025145391406222</v>
       </c>
       <c r="C11">
         <f t="shared" ref="C11:H11" si="2">C7/C4</f>
-        <v>3.1367907399001358</v>
+        <v>3.8090205418279246</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>2.8743944569895583</v>
+        <v>4.0525514954693076</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>2.5026189860320747</v>
+        <v>3.5842761449953526</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>2.5932260174534552</v>
+        <v>3.5236319499283439</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>3.4987655884028617</v>
+        <v>3.3369411825632129</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>3.9402074531811593</v>
+        <v>3.0795776850324068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>